<commit_message>
TS 4.5,4.7 New Stats - 29/03/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.5 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79645276-2BEA-4888-97E5-0E37E590C16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D8F3D9-D531-430F-AF56-19639C718510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3558,10 +3558,10 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Y1235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="O152" sqref="O152"/>
+      <selection pane="bottomLeft" activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -10973,7 +10973,7 @@
       <c r="X151" s="8"/>
       <c r="Y151" s="8"/>
     </row>
-    <row r="152" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B152" s="66" t="s">
         <v>913</v>
       </c>
@@ -11019,7 +11019,7 @@
       <c r="X152" s="8"/>
       <c r="Y152" s="8"/>
     </row>
-    <row r="153" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B153" s="66" t="s">
         <v>913</v>
       </c>
@@ -11064,7 +11064,7 @@
       <c r="X153" s="8"/>
       <c r="Y153" s="8"/>
     </row>
-    <row r="154" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B154" s="66" t="s">
         <v>913</v>
       </c>
@@ -11113,7 +11113,7 @@
       <c r="X154" s="8"/>
       <c r="Y154" s="8"/>
     </row>
-    <row r="155" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B155" s="66" t="s">
         <v>913</v>
       </c>
@@ -11162,7 +11162,7 @@
       <c r="X155" s="8"/>
       <c r="Y155" s="8"/>
     </row>
-    <row r="156" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B156" s="66" t="s">
         <v>913</v>
       </c>
@@ -11211,7 +11211,7 @@
       <c r="X156" s="8"/>
       <c r="Y156" s="8"/>
     </row>
-    <row r="157" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B157" s="66" t="s">
         <v>913</v>
       </c>
@@ -11256,7 +11256,7 @@
       <c r="X157" s="8"/>
       <c r="Y157" s="8"/>
     </row>
-    <row r="158" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B158" s="66" t="s">
         <v>913</v>
       </c>
@@ -11301,7 +11301,7 @@
       <c r="X158" s="8"/>
       <c r="Y158" s="8"/>
     </row>
-    <row r="159" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B159" s="66" t="s">
         <v>913</v>
       </c>
@@ -11350,7 +11350,7 @@
       <c r="X159" s="8"/>
       <c r="Y159" s="8"/>
     </row>
-    <row r="160" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B160" s="66" t="s">
         <v>913</v>
       </c>
@@ -11401,7 +11401,7 @@
       <c r="X160" s="8"/>
       <c r="Y160" s="8"/>
     </row>
-    <row r="161" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B161" s="66" t="s">
         <v>913</v>
       </c>
@@ -11450,7 +11450,7 @@
       <c r="X161" s="8"/>
       <c r="Y161" s="8"/>
     </row>
-    <row r="162" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B162" s="66" t="s">
         <v>913</v>
       </c>
@@ -11495,7 +11495,7 @@
       <c r="X162" s="8"/>
       <c r="Y162" s="8"/>
     </row>
-    <row r="163" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B163" s="66" t="s">
         <v>913</v>
       </c>
@@ -11540,7 +11540,7 @@
       <c r="X163" s="8"/>
       <c r="Y163" s="8"/>
     </row>
-    <row r="164" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B164" s="66" t="s">
         <v>913</v>
       </c>
@@ -11585,7 +11585,7 @@
       <c r="X164" s="8"/>
       <c r="Y164" s="8"/>
     </row>
-    <row r="165" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B165" s="66" t="s">
         <v>913</v>
       </c>
@@ -11630,7 +11630,7 @@
       <c r="X165" s="8"/>
       <c r="Y165" s="8"/>
     </row>
-    <row r="166" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B166" s="66" t="s">
         <v>913</v>
       </c>
@@ -11679,7 +11679,7 @@
       <c r="X166" s="8"/>
       <c r="Y166" s="8"/>
     </row>
-    <row r="167" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B167" s="66" t="s">
         <v>913</v>
       </c>
@@ -11728,7 +11728,7 @@
       <c r="X167" s="8"/>
       <c r="Y167" s="8"/>
     </row>
-    <row r="168" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B168" s="66" t="s">
         <v>913</v>
       </c>
@@ -11777,7 +11777,7 @@
       <c r="X168" s="8"/>
       <c r="Y168" s="8"/>
     </row>
-    <row r="169" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B169" s="66" t="s">
         <v>913</v>
       </c>
@@ -11822,7 +11822,7 @@
       <c r="X169" s="8"/>
       <c r="Y169" s="8"/>
     </row>
-    <row r="170" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B170" s="66" t="s">
         <v>913</v>
       </c>
@@ -11867,7 +11867,7 @@
       <c r="X170" s="8"/>
       <c r="Y170" s="8"/>
     </row>
-    <row r="171" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B171" s="66" t="s">
         <v>913</v>
       </c>
@@ -11916,7 +11916,7 @@
       <c r="X171" s="8"/>
       <c r="Y171" s="8"/>
     </row>
-    <row r="172" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B172" s="66" t="s">
         <v>913</v>
       </c>
@@ -11971,7 +11971,7 @@
       <c r="X172" s="8"/>
       <c r="Y172" s="8"/>
     </row>
-    <row r="173" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B173" s="66" t="s">
         <v>913</v>
       </c>
@@ -12020,7 +12020,7 @@
       <c r="X173" s="8"/>
       <c r="Y173" s="8"/>
     </row>
-    <row r="174" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B174" s="66" t="s">
         <v>913</v>
       </c>
@@ -12067,7 +12067,7 @@
       <c r="X174" s="8"/>
       <c r="Y174" s="8"/>
     </row>
-    <row r="175" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B175" s="66" t="s">
         <v>913</v>
       </c>
@@ -12116,7 +12116,7 @@
       <c r="X175" s="8"/>
       <c r="Y175" s="8"/>
     </row>
-    <row r="176" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B176" s="66" t="s">
         <v>913</v>
       </c>
@@ -12163,7 +12163,7 @@
       <c r="X176" s="8"/>
       <c r="Y176" s="8"/>
     </row>
-    <row r="177" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B177" s="66" t="s">
         <v>913</v>
       </c>
@@ -12210,7 +12210,7 @@
       <c r="X177" s="8"/>
       <c r="Y177" s="8"/>
     </row>
-    <row r="178" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B178" s="66" t="s">
         <v>913</v>
       </c>
@@ -12257,7 +12257,7 @@
       <c r="X178" s="8"/>
       <c r="Y178" s="8"/>
     </row>
-    <row r="179" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B179" s="66" t="s">
         <v>913</v>
       </c>
@@ -12310,7 +12310,7 @@
       <c r="X179" s="8"/>
       <c r="Y179" s="8"/>
     </row>
-    <row r="180" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B180" s="66" t="s">
         <v>913</v>
       </c>
@@ -12355,7 +12355,7 @@
       <c r="X180" s="8"/>
       <c r="Y180" s="8"/>
     </row>
-    <row r="181" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B181" s="66" t="s">
         <v>913</v>
       </c>
@@ -12400,7 +12400,7 @@
       <c r="X181" s="8"/>
       <c r="Y181" s="8"/>
     </row>
-    <row r="182" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B182" s="66" t="s">
         <v>913</v>
       </c>
@@ -12445,7 +12445,7 @@
       <c r="X182" s="8"/>
       <c r="Y182" s="8"/>
     </row>
-    <row r="183" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B183" s="66" t="s">
         <v>913</v>
       </c>
@@ -12494,7 +12494,7 @@
       <c r="X183" s="8"/>
       <c r="Y183" s="8"/>
     </row>
-    <row r="184" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B184" s="66" t="s">
         <v>913</v>
       </c>
@@ -12539,7 +12539,7 @@
       <c r="X184" s="8"/>
       <c r="Y184" s="8"/>
     </row>
-    <row r="185" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B185" s="66" t="s">
         <v>913</v>
       </c>
@@ -12584,7 +12584,7 @@
       <c r="X185" s="8"/>
       <c r="Y185" s="8"/>
     </row>
-    <row r="186" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B186" s="66" t="s">
         <v>913</v>
       </c>
@@ -12629,7 +12629,7 @@
       <c r="X186" s="8"/>
       <c r="Y186" s="8"/>
     </row>
-    <row r="187" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B187" s="66" t="s">
         <v>913</v>
       </c>
@@ -12678,7 +12678,7 @@
       <c r="X187" s="8"/>
       <c r="Y187" s="8"/>
     </row>
-    <row r="188" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B188" s="66" t="s">
         <v>913</v>
       </c>
@@ -12723,7 +12723,7 @@
       <c r="X188" s="8"/>
       <c r="Y188" s="8"/>
     </row>
-    <row r="189" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B189" s="66" t="s">
         <v>913</v>
       </c>
@@ -12770,7 +12770,7 @@
       <c r="X189" s="8"/>
       <c r="Y189" s="8"/>
     </row>
-    <row r="190" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B190" s="66" t="s">
         <v>913</v>
       </c>
@@ -12815,7 +12815,7 @@
       <c r="X190" s="8"/>
       <c r="Y190" s="8"/>
     </row>
-    <row r="191" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B191" s="66" t="s">
         <v>913</v>
       </c>
@@ -12860,7 +12860,7 @@
       <c r="X191" s="8"/>
       <c r="Y191" s="8"/>
     </row>
-    <row r="192" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B192" s="66" t="s">
         <v>913</v>
       </c>
@@ -12905,7 +12905,7 @@
       <c r="X192" s="8"/>
       <c r="Y192" s="8"/>
     </row>
-    <row r="193" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B193" s="66" t="s">
         <v>913</v>
       </c>
@@ -12956,7 +12956,7 @@
       <c r="X193" s="8"/>
       <c r="Y193" s="8"/>
     </row>
-    <row r="194" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B194" s="66" t="s">
         <v>913</v>
       </c>
@@ -13005,7 +13005,7 @@
       <c r="X194" s="8"/>
       <c r="Y194" s="8"/>
     </row>
-    <row r="195" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B195" s="66" t="s">
         <v>913</v>
       </c>
@@ -13052,7 +13052,7 @@
       <c r="X195" s="8"/>
       <c r="Y195" s="8"/>
     </row>
-    <row r="196" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B196" s="66" t="s">
         <v>913</v>
       </c>
@@ -13099,7 +13099,7 @@
       <c r="X196" s="8"/>
       <c r="Y196" s="8"/>
     </row>
-    <row r="197" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B197" s="66" t="s">
         <v>913</v>
       </c>
@@ -13150,7 +13150,7 @@
       <c r="X197" s="8"/>
       <c r="Y197" s="8"/>
     </row>
-    <row r="198" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B198" s="66" t="s">
         <v>913</v>
       </c>
@@ -13197,7 +13197,7 @@
       <c r="X198" s="8"/>
       <c r="Y198" s="8"/>
     </row>
-    <row r="199" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B199" s="66" t="s">
         <v>913</v>
       </c>
@@ -13248,7 +13248,7 @@
       <c r="X199" s="8"/>
       <c r="Y199" s="8"/>
     </row>
-    <row r="200" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B200" s="66" t="s">
         <v>913</v>
       </c>
@@ -13299,7 +13299,7 @@
       <c r="X200" s="8"/>
       <c r="Y200" s="8"/>
     </row>
-    <row r="201" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B201" s="66" t="s">
         <v>913</v>
       </c>
@@ -13344,7 +13344,7 @@
       <c r="X201" s="8"/>
       <c r="Y201" s="8"/>
     </row>
-    <row r="202" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B202" s="66" t="s">
         <v>913</v>
       </c>
@@ -13389,7 +13389,7 @@
       <c r="X202" s="8"/>
       <c r="Y202" s="8"/>
     </row>
-    <row r="203" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B203" s="66" t="s">
         <v>913</v>
       </c>
@@ -13434,7 +13434,7 @@
       <c r="X203" s="8"/>
       <c r="Y203" s="8"/>
     </row>
-    <row r="204" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B204" s="66" t="s">
         <v>913</v>
       </c>
@@ -13479,7 +13479,7 @@
       <c r="X204" s="8"/>
       <c r="Y204" s="8"/>
     </row>
-    <row r="205" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B205" s="66" t="s">
         <v>913</v>
       </c>
@@ -13528,7 +13528,7 @@
       <c r="X205" s="8"/>
       <c r="Y205" s="8"/>
     </row>
-    <row r="206" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B206" s="66" t="s">
         <v>913</v>
       </c>
@@ -13573,7 +13573,7 @@
       <c r="X206" s="8"/>
       <c r="Y206" s="8"/>
     </row>
-    <row r="207" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B207" s="66" t="s">
         <v>913</v>
       </c>
@@ -13622,7 +13622,7 @@
       <c r="X207" s="8"/>
       <c r="Y207" s="8"/>
     </row>
-    <row r="208" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B208" s="66" t="s">
         <v>913</v>
       </c>
@@ -13668,7 +13668,7 @@
       <c r="X208" s="8"/>
       <c r="Y208" s="8"/>
     </row>
-    <row r="209" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B209" s="66" t="s">
         <v>913</v>
       </c>
@@ -13713,7 +13713,7 @@
       <c r="X209" s="8"/>
       <c r="Y209" s="8"/>
     </row>
-    <row r="210" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B210" s="66" t="s">
         <v>913</v>
       </c>
@@ -13758,7 +13758,7 @@
       <c r="X210" s="8"/>
       <c r="Y210" s="8"/>
     </row>
-    <row r="211" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B211" s="66" t="s">
         <v>913</v>
       </c>
@@ -13803,7 +13803,7 @@
       <c r="X211" s="8"/>
       <c r="Y211" s="8"/>
     </row>
-    <row r="212" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B212" s="66" t="s">
         <v>913</v>
       </c>
@@ -13848,7 +13848,7 @@
       <c r="X212" s="8"/>
       <c r="Y212" s="8"/>
     </row>
-    <row r="213" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B213" s="66" t="s">
         <v>913</v>
       </c>
@@ -13893,7 +13893,7 @@
       <c r="X213" s="8"/>
       <c r="Y213" s="8"/>
     </row>
-    <row r="214" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B214" s="66" t="s">
         <v>913</v>
       </c>
@@ -13942,7 +13942,7 @@
       <c r="X214" s="8"/>
       <c r="Y214" s="8"/>
     </row>
-    <row r="215" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B215" s="66" t="s">
         <v>913</v>
       </c>
@@ -13997,7 +13997,7 @@
       <c r="X215" s="8"/>
       <c r="Y215" s="8"/>
     </row>
-    <row r="216" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B216" s="66" t="s">
         <v>913</v>
       </c>
@@ -14048,7 +14048,7 @@
       <c r="X216" s="8"/>
       <c r="Y216" s="8"/>
     </row>
-    <row r="217" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B217" s="66" t="s">
         <v>913</v>
       </c>
@@ -14099,7 +14099,7 @@
       <c r="X217" s="8"/>
       <c r="Y217" s="8"/>
     </row>
-    <row r="218" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B218" s="66" t="s">
         <v>913</v>
       </c>
@@ -14146,7 +14146,7 @@
       <c r="X218" s="8"/>
       <c r="Y218" s="8"/>
     </row>
-    <row r="219" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B219" s="66" t="s">
         <v>913</v>
       </c>
@@ -14193,7 +14193,7 @@
       <c r="X219" s="8"/>
       <c r="Y219" s="8"/>
     </row>
-    <row r="220" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B220" s="66" t="s">
         <v>913</v>
       </c>
@@ -14240,7 +14240,7 @@
       <c r="X220" s="8"/>
       <c r="Y220" s="8"/>
     </row>
-    <row r="221" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B221" s="66" t="s">
         <v>913</v>
       </c>
@@ -14287,7 +14287,7 @@
       <c r="X221" s="8"/>
       <c r="Y221" s="8"/>
     </row>
-    <row r="222" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B222" s="66" t="s">
         <v>913</v>
       </c>
@@ -14332,7 +14332,7 @@
       <c r="X222" s="8"/>
       <c r="Y222" s="8"/>
     </row>
-    <row r="223" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B223" s="66" t="s">
         <v>913</v>
       </c>
@@ -53229,7 +53229,7 @@
       <c r="X1179" s="8"/>
       <c r="Y1179" s="8"/>
     </row>
-    <row r="1180" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1180" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1180" s="25"/>
       <c r="F1180" s="25"/>
       <c r="G1180" s="25"/>
@@ -53270,7 +53270,7 @@
       <c r="X1180" s="8"/>
       <c r="Y1180" s="8"/>
     </row>
-    <row r="1181" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1181" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1181" s="25"/>
       <c r="F1181" s="25"/>
       <c r="G1181" s="25"/>
@@ -53312,7 +53312,7 @@
       <c r="X1181" s="8"/>
       <c r="Y1181" s="8"/>
     </row>
-    <row r="1182" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1182" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1182" s="25"/>
       <c r="F1182" s="25"/>
       <c r="G1182" s="25"/>
@@ -53356,7 +53356,7 @@
       <c r="X1182" s="8"/>
       <c r="Y1182" s="8"/>
     </row>
-    <row r="1183" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1183" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1183" s="25"/>
       <c r="F1183" s="25"/>
       <c r="G1183" s="25"/>
@@ -53396,7 +53396,7 @@
       <c r="X1183" s="8"/>
       <c r="Y1183" s="8"/>
     </row>
-    <row r="1184" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1184" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1184" s="25"/>
       <c r="F1184" s="25"/>
       <c r="G1184" s="25"/>
@@ -53436,7 +53436,7 @@
       <c r="X1184" s="8"/>
       <c r="Y1184" s="8"/>
     </row>
-    <row r="1185" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1185" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1185" s="25"/>
       <c r="F1185" s="25"/>
       <c r="G1185" s="25"/>
@@ -53476,7 +53476,7 @@
       <c r="X1185" s="8"/>
       <c r="Y1185" s="8"/>
     </row>
-    <row r="1186" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1186" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1186" s="25"/>
       <c r="F1186" s="25"/>
       <c r="G1186" s="25"/>
@@ -53515,7 +53515,7 @@
       <c r="X1186" s="8"/>
       <c r="Y1186" s="8"/>
     </row>
-    <row r="1187" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1187" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1187" s="25"/>
       <c r="F1187" s="25"/>
       <c r="G1187" s="25"/>
@@ -53554,7 +53554,7 @@
       <c r="X1187" s="8"/>
       <c r="Y1187" s="8"/>
     </row>
-    <row r="1188" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1188" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1188" s="25"/>
       <c r="F1188" s="25"/>
       <c r="G1188" s="25"/>
@@ -53593,7 +53593,7 @@
       <c r="X1188" s="8"/>
       <c r="Y1188" s="8"/>
     </row>
-    <row r="1189" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1189" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1189" s="25"/>
       <c r="F1189" s="25"/>
       <c r="G1189" s="25"/>
@@ -53630,7 +53630,7 @@
       <c r="X1189" s="8"/>
       <c r="Y1189" s="8"/>
     </row>
-    <row r="1190" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1190" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1190" s="25"/>
       <c r="F1190" s="25"/>
       <c r="G1190" s="25"/>
@@ -53674,7 +53674,7 @@
       <c r="X1190" s="8"/>
       <c r="Y1190" s="8"/>
     </row>
-    <row r="1191" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1191" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1191" s="25"/>
       <c r="F1191" s="25"/>
       <c r="G1191" s="25"/>
@@ -53711,7 +53711,7 @@
       <c r="X1191" s="8"/>
       <c r="Y1191" s="8"/>
     </row>
-    <row r="1192" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1192" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1192" s="25"/>
       <c r="F1192" s="25"/>
       <c r="G1192" s="25"/>
@@ -53753,7 +53753,7 @@
       <c r="X1192" s="8"/>
       <c r="Y1192" s="8"/>
     </row>
-    <row r="1193" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1193" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1193" s="25"/>
       <c r="F1193" s="25"/>
       <c r="G1193" s="25"/>
@@ -53793,7 +53793,7 @@
       <c r="X1193" s="8"/>
       <c r="Y1193" s="8"/>
     </row>
-    <row r="1194" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1194" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1194" s="25"/>
       <c r="F1194" s="25"/>
       <c r="G1194" s="25"/>
@@ -53830,7 +53830,7 @@
       <c r="X1194" s="8"/>
       <c r="Y1194" s="8"/>
     </row>
-    <row r="1195" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1195" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1195" s="25"/>
       <c r="F1195" s="25"/>
       <c r="G1195" s="25"/>
@@ -53871,7 +53871,7 @@
       <c r="X1195" s="8"/>
       <c r="Y1195" s="8"/>
     </row>
-    <row r="1196" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1196" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1196" s="25"/>
       <c r="F1196" s="25"/>
       <c r="G1196" s="25"/>
@@ -53908,7 +53908,7 @@
       <c r="X1196" s="8"/>
       <c r="Y1196" s="8"/>
     </row>
-    <row r="1197" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1197" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1197" s="25"/>
       <c r="F1197" s="25"/>
       <c r="G1197" s="25"/>
@@ -53945,7 +53945,7 @@
       <c r="X1197" s="8"/>
       <c r="Y1197" s="8"/>
     </row>
-    <row r="1198" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1198" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1198" s="25"/>
       <c r="F1198" s="25"/>
       <c r="G1198" s="25"/>
@@ -53982,7 +53982,7 @@
       <c r="X1198" s="8"/>
       <c r="Y1198" s="8"/>
     </row>
-    <row r="1199" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1199" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1199" s="25"/>
       <c r="F1199" s="25"/>
       <c r="G1199" s="25"/>
@@ -54019,7 +54019,7 @@
       <c r="X1199" s="8"/>
       <c r="Y1199" s="8"/>
     </row>
-    <row r="1200" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1200" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1200" s="25"/>
       <c r="F1200" s="25"/>
       <c r="G1200" s="25"/>
@@ -54058,7 +54058,7 @@
       <c r="X1200" s="8"/>
       <c r="Y1200" s="8"/>
     </row>
-    <row r="1201" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1201" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1201" s="25"/>
       <c r="F1201" s="25"/>
       <c r="G1201" s="25"/>
@@ -54097,7 +54097,7 @@
       <c r="X1201" s="8"/>
       <c r="Y1201" s="8"/>
     </row>
-    <row r="1202" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1202" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1202" s="25"/>
       <c r="F1202" s="25"/>
       <c r="G1202" s="25"/>
@@ -54136,7 +54136,7 @@
       <c r="X1202" s="8"/>
       <c r="Y1202" s="8"/>
     </row>
-    <row r="1203" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1203" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1203" s="25"/>
       <c r="F1203" s="25"/>
       <c r="G1203" s="25"/>
@@ -54175,7 +54175,7 @@
       <c r="X1203" s="8"/>
       <c r="Y1203" s="8"/>
     </row>
-    <row r="1204" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1204" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1204" s="25"/>
       <c r="F1204" s="25"/>
       <c r="G1204" s="25"/>
@@ -54214,7 +54214,7 @@
       <c r="X1204" s="8"/>
       <c r="Y1204" s="8"/>
     </row>
-    <row r="1205" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1205" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1205" s="25"/>
       <c r="F1205" s="25"/>
       <c r="G1205" s="25"/>
@@ -54251,7 +54251,7 @@
       <c r="X1205" s="8"/>
       <c r="Y1205" s="8"/>
     </row>
-    <row r="1206" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1206" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1206" s="25"/>
       <c r="F1206" s="25"/>
       <c r="G1206" s="25"/>
@@ -54289,7 +54289,7 @@
       <c r="X1206" s="8"/>
       <c r="Y1206" s="8"/>
     </row>
-    <row r="1207" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1207" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1207" s="25"/>
       <c r="F1207" s="25"/>
       <c r="G1207" s="25"/>
@@ -54327,7 +54327,7 @@
       <c r="X1207" s="8"/>
       <c r="Y1207" s="8"/>
     </row>
-    <row r="1208" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1208" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1208" s="25"/>
       <c r="F1208" s="25"/>
       <c r="G1208" s="25"/>
@@ -54365,7 +54365,7 @@
       <c r="X1208" s="8"/>
       <c r="Y1208" s="8"/>
     </row>
-    <row r="1209" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1209" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1209" s="25"/>
       <c r="F1209" s="25"/>
       <c r="G1209" s="25"/>
@@ -54403,7 +54403,7 @@
       <c r="X1209" s="8"/>
       <c r="Y1209" s="8"/>
     </row>
-    <row r="1210" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1210" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1210" s="25"/>
       <c r="F1210" s="25"/>
       <c r="G1210" s="25"/>
@@ -54441,7 +54441,7 @@
       <c r="X1210" s="8"/>
       <c r="Y1210" s="8"/>
     </row>
-    <row r="1211" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1211" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1211" s="25"/>
       <c r="F1211" s="25"/>
       <c r="G1211" s="25"/>
@@ -54479,7 +54479,7 @@
       <c r="X1211" s="8"/>
       <c r="Y1211" s="8"/>
     </row>
-    <row r="1212" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1212" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1212" s="25"/>
       <c r="F1212" s="25"/>
       <c r="G1212" s="25"/>
@@ -54517,7 +54517,7 @@
       <c r="X1212" s="8"/>
       <c r="Y1212" s="8"/>
     </row>
-    <row r="1213" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1213" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1213" s="25"/>
       <c r="F1213" s="25"/>
       <c r="G1213" s="25"/>
@@ -54555,7 +54555,7 @@
       <c r="X1213" s="8"/>
       <c r="Y1213" s="8"/>
     </row>
-    <row r="1214" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1214" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1214" s="25"/>
       <c r="F1214" s="25"/>
       <c r="G1214" s="25"/>
@@ -54593,7 +54593,7 @@
       <c r="X1214" s="8"/>
       <c r="Y1214" s="8"/>
     </row>
-    <row r="1215" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1215" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1215" s="25"/>
       <c r="F1215" s="25"/>
       <c r="G1215" s="25"/>
@@ -54631,7 +54631,7 @@
       <c r="X1215" s="8"/>
       <c r="Y1215" s="8"/>
     </row>
-    <row r="1216" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1216" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1216" s="25"/>
       <c r="F1216" s="25"/>
       <c r="G1216" s="25"/>
@@ -54669,7 +54669,7 @@
       <c r="X1216" s="8"/>
       <c r="Y1216" s="8"/>
     </row>
-    <row r="1217" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1217" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1217" s="25"/>
       <c r="F1217" s="25"/>
       <c r="G1217" s="25"/>
@@ -54706,7 +54706,7 @@
       <c r="X1217" s="8"/>
       <c r="Y1217" s="8"/>
     </row>
-    <row r="1218" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1218" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1218" s="25"/>
       <c r="F1218" s="25"/>
       <c r="G1218" s="25"/>
@@ -54743,7 +54743,7 @@
       <c r="X1218" s="8"/>
       <c r="Y1218" s="8"/>
     </row>
-    <row r="1219" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1219" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1219" s="25"/>
       <c r="F1219" s="25"/>
       <c r="G1219" s="25"/>
@@ -54780,7 +54780,7 @@
       <c r="X1219" s="8"/>
       <c r="Y1219" s="8"/>
     </row>
-    <row r="1220" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1220" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1220" s="25"/>
       <c r="F1220" s="25"/>
       <c r="G1220" s="25"/>
@@ -54817,7 +54817,7 @@
       <c r="X1220" s="8"/>
       <c r="Y1220" s="8"/>
     </row>
-    <row r="1221" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1221" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1221" s="25"/>
       <c r="F1221" s="25"/>
       <c r="G1221" s="25"/>
@@ -54854,7 +54854,7 @@
       <c r="X1221" s="8"/>
       <c r="Y1221" s="8"/>
     </row>
-    <row r="1222" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1222" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1222" s="25"/>
       <c r="F1222" s="25"/>
       <c r="G1222" s="25"/>
@@ -54891,7 +54891,7 @@
       <c r="X1222" s="8"/>
       <c r="Y1222" s="8"/>
     </row>
-    <row r="1223" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1223" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1223" s="25"/>
       <c r="F1223" s="25"/>
       <c r="G1223" s="25"/>
@@ -54928,7 +54928,7 @@
       <c r="X1223" s="8"/>
       <c r="Y1223" s="8"/>
     </row>
-    <row r="1224" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1224" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1224" s="25"/>
       <c r="F1224" s="25"/>
       <c r="G1224" s="25"/>
@@ -54965,7 +54965,7 @@
       <c r="X1224" s="8"/>
       <c r="Y1224" s="8"/>
     </row>
-    <row r="1225" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1225" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1225" s="25"/>
       <c r="F1225" s="25"/>
       <c r="G1225" s="25"/>
@@ -55002,7 +55002,7 @@
       <c r="X1225" s="8"/>
       <c r="Y1225" s="8"/>
     </row>
-    <row r="1226" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1226" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1226" s="25"/>
       <c r="F1226" s="25"/>
       <c r="G1226" s="25"/>
@@ -55039,7 +55039,7 @@
       <c r="X1226" s="8"/>
       <c r="Y1226" s="8"/>
     </row>
-    <row r="1227" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1227" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1227" s="25"/>
       <c r="F1227" s="25"/>
       <c r="G1227" s="25"/>
@@ -55076,7 +55076,7 @@
       <c r="X1227" s="8"/>
       <c r="Y1227" s="8"/>
     </row>
-    <row r="1228" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1228" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1228" s="25"/>
       <c r="F1228" s="25"/>
       <c r="G1228" s="25"/>
@@ -55113,7 +55113,7 @@
       <c r="X1228" s="8"/>
       <c r="Y1228" s="8"/>
     </row>
-    <row r="1229" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1229" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1229" s="25"/>
       <c r="F1229" s="25"/>
       <c r="G1229" s="25"/>
@@ -55150,7 +55150,7 @@
       <c r="X1229" s="8"/>
       <c r="Y1229" s="8"/>
     </row>
-    <row r="1230" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1230" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1230" s="25"/>
       <c r="F1230" s="25"/>
       <c r="G1230" s="25"/>
@@ -55188,7 +55188,7 @@
       <c r="X1230" s="8"/>
       <c r="Y1230" s="8"/>
     </row>
-    <row r="1231" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1231" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1231" s="25"/>
       <c r="F1231" s="25"/>
       <c r="G1231" s="25"/>
@@ -55226,7 +55226,7 @@
       <c r="X1231" s="8"/>
       <c r="Y1231" s="8"/>
     </row>
-    <row r="1232" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1232" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1232" s="25"/>
       <c r="F1232" s="25"/>
       <c r="G1232" s="25"/>
@@ -55264,7 +55264,7 @@
       <c r="X1232" s="8"/>
       <c r="Y1232" s="8"/>
     </row>
-    <row r="1233" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1233" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1233" s="25"/>
       <c r="F1233" s="25"/>
       <c r="G1233" s="25"/>
@@ -55302,7 +55302,7 @@
       <c r="X1233" s="8"/>
       <c r="Y1233" s="8"/>
     </row>
-    <row r="1234" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1234" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1234" s="25"/>
       <c r="F1234" s="25"/>
       <c r="G1234" s="25"/>
@@ -55340,7 +55340,7 @@
       <c r="X1234" s="8"/>
       <c r="Y1234" s="8"/>
     </row>
-    <row r="1235" spans="5:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1235" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1235" s="25"/>
       <c r="F1235" s="25"/>
       <c r="G1235" s="25"/>
@@ -55386,7 +55386,7 @@
   <autoFilter ref="B1:V1235" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="7">
       <filters>
-        <filter val="4.5.1.4"/>
+        <filter val="4.5.11.2"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>